<commit_message>
Prepare for plotting K theory
</commit_message>
<xml_diff>
--- a/TestData_K/K_68Bus_IBR.xlsx
+++ b/TestData_K/K_68Bus_IBR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-Communication-Isomorphism\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-Communication-Isomorphism\TestData_K\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2B7194-046D-4438-B2E8-E95EBFB69F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92CF7FD-73E4-4CAB-B4F2-DD4DC8BE62FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -647,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -3297,7 +3297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -4600,8 +4600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>